<commit_message>
test commit rmi-data branch
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\RMI_all_states\AL\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF1F323B-1FA0-4E89-AD48-2CCFDCA8473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{090F52D1-FA34-40C1-9F47-BA16047A9233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="720" windowWidth="13920" windowHeight="16590" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="285" windowWidth="15915" windowHeight="16410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,7 +903,7 @@
         <v>91</v>
       </c>
       <c r="C1" s="5">
-        <v>44873</v>
+        <v>44944</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>81</v>
@@ -1392,7 +1392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE11CAF-345E-44DE-959F-9F9638946419}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1913,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2105,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2297,7 +2299,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>3409.5382097277702</v>
+        <v>450</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2306,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1123.4017902722201</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2489,7 +2491,7 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>189.41878942931999</v>
+        <v>72</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2498,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2681,7 +2683,7 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>568.256368287962</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2690,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>187.23363171203701</v>
+        <v>5</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2873,7 +2875,7 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>189.41878942931999</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2882,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -3065,7 +3067,7 @@
         <v>6</v>
       </c>
       <c r="C53">
-        <v>378.837578858641</v>
+        <v>29</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3074,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>124.82242114135801</v>
+        <v>11</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3257,7 +3259,7 @@
         <v>6</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4025,7 +4027,7 @@
         <v>6</v>
       </c>
       <c r="C83">
-        <v>1515.3503154345599</v>
+        <v>279</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -4034,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>499.28968456543299</v>
+        <v>21</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4217,7 +4219,7 @@
         <v>6</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -4793,7 +4795,7 @@
         <v>6</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -4985,7 +4987,7 @@
         <v>6</v>
       </c>
       <c r="C113">
-        <v>947.09394714660402</v>
+        <v>166</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -4994,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="F113">
-        <v>312.05605285339499</v>
+        <v>43</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5177,7 +5179,7 @@
         <v>6</v>
       </c>
       <c r="C119">
-        <v>568.256368287962</v>
+        <v>50</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -5186,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="F119">
-        <v>187.23363171203701</v>
+        <v>5</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5368,16 +5370,10 @@
       <c r="B125" t="s">
         <v>6</v>
       </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
       <c r="D125">
         <v>0</v>
       </c>
       <c r="E125">
-        <v>0</v>
-      </c>
-      <c r="F125">
         <v>0</v>
       </c>
       <c r="G125">
@@ -5561,7 +5557,7 @@
         <v>6</v>
       </c>
       <c r="C131">
-        <v>189.41878942931999</v>
+        <v>5</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -5570,7 +5566,7 @@
         <v>0</v>
       </c>
       <c r="F131">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -5753,7 +5749,7 @@
         <v>6</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -5762,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -5945,7 +5941,7 @@
         <v>6</v>
       </c>
       <c r="C143">
-        <v>189.41878942931999</v>
+        <v>32</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -5954,7 +5950,7 @@
         <v>0</v>
       </c>
       <c r="F143">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G143">
         <v>0</v>
@@ -6521,7 +6517,7 @@
         <v>6</v>
       </c>
       <c r="C161">
-        <v>378.837578858641</v>
+        <v>20</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -6530,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="F161">
-        <v>124.82242114135801</v>
+        <v>0</v>
       </c>
       <c r="G161">
         <v>0</v>
@@ -7289,7 +7285,7 @@
         <v>6</v>
       </c>
       <c r="C185">
-        <v>568.256368287962</v>
+        <v>190</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -7298,7 +7294,7 @@
         <v>0</v>
       </c>
       <c r="F185">
-        <v>187.23363171203701</v>
+        <v>25</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -7490,7 +7486,7 @@
         <v>0</v>
       </c>
       <c r="F191">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -7865,7 +7861,7 @@
         <v>6</v>
       </c>
       <c r="C203">
-        <v>3788.3757885864102</v>
+        <v>835</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -7874,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="F203">
-        <v>1248.22421141358</v>
+        <v>17</v>
       </c>
       <c r="G203">
         <v>0</v>
@@ -8057,7 +8053,7 @@
         <v>6</v>
       </c>
       <c r="C209">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -8249,7 +8245,7 @@
         <v>6</v>
       </c>
       <c r="C215">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D215">
         <v>0</v>
@@ -8441,7 +8437,7 @@
         <v>6</v>
       </c>
       <c r="C221">
-        <v>189.41878942931999</v>
+        <v>72</v>
       </c>
       <c r="D221">
         <v>0</v>
@@ -8450,7 +8446,7 @@
         <v>0</v>
       </c>
       <c r="F221">
-        <v>62.411210570679103</v>
+        <v>1</v>
       </c>
       <c r="G221">
         <v>0</v>
@@ -8633,7 +8629,7 @@
         <v>6</v>
       </c>
       <c r="C227">
-        <v>1894.1878942932001</v>
+        <v>297</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -8642,7 +8638,7 @@
         <v>0</v>
       </c>
       <c r="F227">
-        <v>624.112105706791</v>
+        <v>0</v>
       </c>
       <c r="G227">
         <v>0</v>
@@ -8825,7 +8821,7 @@
         <v>6</v>
       </c>
       <c r="C233">
-        <v>189.41878942931999</v>
+        <v>0</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -8834,7 +8830,7 @@
         <v>0</v>
       </c>
       <c r="F233">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G233">
         <v>0</v>
@@ -9401,7 +9397,7 @@
         <v>6</v>
       </c>
       <c r="C251">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -9410,7 +9406,7 @@
         <v>0</v>
       </c>
       <c r="F251">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -9593,7 +9589,7 @@
         <v>6</v>
       </c>
       <c r="C257">
-        <v>189.41878942931999</v>
+        <v>94</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -9602,7 +9598,7 @@
         <v>0</v>
       </c>
       <c r="F257">
-        <v>62.411210570679103</v>
+        <v>19</v>
       </c>
       <c r="G257">
         <v>0</v>
@@ -9785,7 +9781,7 @@
         <v>6</v>
       </c>
       <c r="C263">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9794,7 +9790,7 @@
         <v>0</v>
       </c>
       <c r="F263">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G263">
         <v>0</v>
@@ -9977,7 +9973,7 @@
         <v>6</v>
       </c>
       <c r="C269">
-        <v>568.256368287962</v>
+        <v>19</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9986,7 +9982,7 @@
         <v>0</v>
       </c>
       <c r="F269">
-        <v>187.23363171203701</v>
+        <v>19</v>
       </c>
       <c r="G269">
         <v>0</v>
@@ -10361,7 +10357,7 @@
         <v>6</v>
       </c>
       <c r="C281">
-        <v>378.837578858641</v>
+        <v>40</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -10370,7 +10366,7 @@
         <v>0</v>
       </c>
       <c r="F281">
-        <v>124.82242114135801</v>
+        <v>2</v>
       </c>
       <c r="G281">
         <v>0</v>
@@ -10553,7 +10549,7 @@
         <v>6</v>
       </c>
       <c r="C287">
-        <v>189.41878942931999</v>
+        <v>4</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -10562,7 +10558,7 @@
         <v>0</v>
       </c>
       <c r="F287">
-        <v>62.411210570679103</v>
+        <v>0</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -11038,7 +11034,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11369,7 +11365,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>